<commit_message>
results of GoodSplit with TeacherRL
</commit_message>
<xml_diff>
--- a/data/DFA_R97_sched4.xlsx
+++ b/data/DFA_R97_sched4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="10515" windowHeight="4695" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="10515" windowHeight="4695"/>
   </bookViews>
   <sheets>
     <sheet name="DFA_R97_sched4" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="59">
   <si>
     <t>Correct;#Resets;#OQs;#EQs;#symbols;fileName;Algorithm;CEprocessing;Teacher;BB;</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>TTT</t>
+  </si>
+  <si>
+    <t>Correct: 1, reset: 350368,      OQ: 350368,     EQ: 0,  symbols: 4772106,</t>
+  </si>
+  <si>
+    <t>GoodSplit</t>
+  </si>
+  <si>
+    <t>maxLen:3</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +1171,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142992128"/>
-        <c:axId val="142993664"/>
+        <c:axId val="204792576"/>
+        <c:axId val="204794112"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1236,11 +1245,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143267712"/>
-        <c:axId val="143265792"/>
+        <c:axId val="205068160"/>
+        <c:axId val="205066240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142992128"/>
+        <c:axId val="204792576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,7 +1258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142993664"/>
+        <c:crossAx val="204794112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1257,7 +1266,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142993664"/>
+        <c:axId val="204794112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,12 +1277,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142992128"/>
+        <c:crossAx val="204792576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143265792"/>
+        <c:axId val="205066240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,19 +1304,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143267712"/>
+        <c:crossAx val="205068160"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="143267712"/>
+        <c:axId val="205068160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,7 +1324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143265792"/>
+        <c:crossAx val="205066240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1326,7 +1334,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1747,8 +1754,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143607296"/>
-        <c:axId val="143608832"/>
+        <c:axId val="205407744"/>
+        <c:axId val="205409280"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1821,11 +1828,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143624832"/>
-        <c:axId val="143622912"/>
+        <c:axId val="205421184"/>
+        <c:axId val="205419264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143607296"/>
+        <c:axId val="205407744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,7 +1841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143608832"/>
+        <c:crossAx val="205409280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1842,7 +1849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143608832"/>
+        <c:axId val="205409280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1853,12 +1860,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143607296"/>
+        <c:crossAx val="205407744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143622912"/>
+        <c:axId val="205419264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,19 +1887,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143624832"/>
+        <c:crossAx val="205421184"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="143624832"/>
+        <c:axId val="205421184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,7 +1907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143622912"/>
+        <c:crossAx val="205419264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1911,7 +1917,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2332,8 +2337,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143329536"/>
-        <c:axId val="143339520"/>
+        <c:axId val="205461760"/>
+        <c:axId val="205471744"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2475,11 +2480,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="149854464"/>
-        <c:axId val="149852160"/>
+        <c:axId val="205474816"/>
+        <c:axId val="205473280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143329536"/>
+        <c:axId val="205461760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2488,7 +2493,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143339520"/>
+        <c:crossAx val="205471744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2496,7 +2501,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143339520"/>
+        <c:axId val="205471744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2507,12 +2512,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143329536"/>
+        <c:crossAx val="205461760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149852160"/>
+        <c:axId val="205473280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2522,12 +2527,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149854464"/>
+        <c:crossAx val="205474816"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="149854464"/>
+        <c:axId val="205474816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2536,7 +2541,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149852160"/>
+        <c:crossAx val="205473280"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2545,7 +2551,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2581,7 +2586,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="82" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2960,10 +2965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4001,7 +4006,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -4030,7 +4035,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -4057,6 +4062,38 @@
       </c>
       <c r="J34" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>350368</v>
+      </c>
+      <c r="C36">
+        <v>350368</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>4772106</v>
+      </c>
+      <c r="F36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I36" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
L* Semantic Suffix Closedness counterexample - Moore_R100_PDS.fsm with TeacherRL
</commit_message>
<xml_diff>
--- a/data/DFA_R97_sched4.xlsx
+++ b/data/DFA_R97_sched4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="10515" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="10515" windowHeight="4695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DFA_R97_sched4" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="TeacherBB" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Moore_R10_PDS" localSheetId="0">DFA_R97_sched4!$A$1:$K$34</definedName>
+    <definedName name="Moore_R10_PDS" localSheetId="0">DFA_R97_sched4!$A$1:$K$41</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -42,91 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="59">
-  <si>
-    <t>Correct;#Resets;#OQs;#EQs;#symbols;fileName;Algorithm;CEprocessing;Teacher;BB;</t>
-  </si>
-  <si>
-    <t>1;456;912;5;2598;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addAllPrefixesToS;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;342;677;8;1363;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffixAfterLastStateToE;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;328;656;8;1324;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addAllSuffixesAfterLastStateToE;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;328;656;8;1324;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffix1by1ToE;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;339;678;8;1356;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffixToE_binarySearch;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;260;521;9;1063;../data/tests/sequences/Moore_R10_PDS.fsm;DT;;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;621;1237;3;3009;../data/tests/sequences/Moore_R10_PDS.fsm;OP;AllGlobally;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;504;999;5;2342;../data/tests/sequences/Moore_R10_PDS.fsm;OP;OneGlobally;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;379;749;5;1586;../data/tests/sequences/Moore_R10_PDS.fsm;OP;OneLocally;TeacherDFSM;;</t>
-  </si>
-  <si>
-    <t>1;585;1170;6;3360;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addAllPrefixesToS;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;385;762;9;1513;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffixAfterLastStateToE;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;369;738;9;1469;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addAllSuffixesAfterLastStateToE;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;369;738;9;1469;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffix1by1ToE;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;382;764;9;1506;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffixToE_binarySearch;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;260;521;9;1063;../data/tests/sequences/Moore_R10_PDS.fsm;DT;;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;905;1805;5;5016;../data/tests/sequences/Moore_R10_PDS.fsm;OP;AllGlobally;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;504;999;5;2342;../data/tests/sequences/Moore_R10_PDS.fsm;OP;OneGlobally;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;379;749;5;1586;../data/tests/sequences/Moore_R10_PDS.fsm;OP;OneLocally;TeacherRL;;</t>
-  </si>
-  <si>
-    <t>1;1515;1040;6;7288;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addAllPrefixesToS;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
-  <si>
-    <t>1;1418;592;7;7940;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffixAfterLastStateToE;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
-  <si>
-    <t>1;1529;820;7;7940;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addAllSuffixesAfterLastStateToE;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
-  <si>
-    <t>1;1529;820;7;7940;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffix1by1ToE;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
-  <si>
-    <t>1;1422;606;7;7940;../data/tests/sequences/Moore_R10_PDS.fsm;L*;addSuffixToE_binarySearch;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
-  <si>
-    <t>1;1343;517;9;7726;../data/tests/sequences/Moore_R10_PDS.fsm;DT;;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
-  <si>
-    <t>1;1838;1655;3;8395;../data/tests/sequences/Moore_R10_PDS.fsm;OP;AllGlobally;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
-  <si>
-    <t>1;1596;1015;5;8336;../data/tests/sequences/Moore_R10_PDS.fsm;OP;OneGlobally;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
-  <si>
-    <t>1;1472;767;5;8181;../data/tests/sequences/Moore_R10_PDS.fsm;OP;OneLocally;TeacherBB:SPY_method (3 extra states);BlackBoxDFSM;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="33">
   <si>
     <t>Correct</t>
   </si>
@@ -212,13 +128,19 @@
     <t>TTT</t>
   </si>
   <si>
-    <t>Correct: 1, reset: 350368,      OQ: 350368,     EQ: 0,  symbols: 4772106,</t>
-  </si>
-  <si>
     <t>GoodSplit</t>
   </si>
   <si>
-    <t>maxLen:3</t>
+    <t>maxDistLen:2</t>
+  </si>
+  <si>
+    <t>OTree</t>
+  </si>
+  <si>
+    <t>ExtraStates:1</t>
+  </si>
+  <si>
+    <t>maxDistLen:3</t>
   </si>
 </sst>
 </file>
@@ -796,9 +718,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$2:$H$12</c:f>
+              <c:f>DFA_R97_sched4!$G$2:$H$14</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -824,6 +746,12 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -858,6 +786,12 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -865,10 +799,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$B$2:$B$12</c:f>
+              <c:f>DFA_R97_sched4!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>23235</c:v>
                 </c:pt>
@@ -901,6 +835,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>16740</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148038</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,9 +863,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$2:$H$12</c:f>
+              <c:f>DFA_R97_sched4!$G$2:$H$14</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -951,6 +891,12 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -985,6 +931,12 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -992,10 +944,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$C$2:$C$12</c:f>
+              <c:f>DFA_R97_sched4!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>23235</c:v>
                 </c:pt>
@@ -1028,6 +980,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>16741</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148038</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1050,9 +1008,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$2:$H$12</c:f>
+              <c:f>DFA_R97_sched4!$G$2:$H$14</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -1078,6 +1036,12 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1112,6 +1076,12 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1119,10 +1089,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$E$2:$E$12</c:f>
+              <c:f>DFA_R97_sched4!$E$2:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>306248</c:v>
                 </c:pt>
@@ -1155,6 +1125,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>223978</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1916339</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>193827</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1171,8 +1147,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="204792576"/>
-        <c:axId val="204794112"/>
+        <c:axId val="231966592"/>
+        <c:axId val="204678272"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1193,10 +1169,10 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$D$2:$D$12</c:f>
+              <c:f>DFA_R97_sched4!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
                 </c:pt>
@@ -1229,6 +1205,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1245,11 +1227,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="205068160"/>
-        <c:axId val="205066240"/>
+        <c:axId val="204681984"/>
+        <c:axId val="204679808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="204792576"/>
+        <c:axId val="231966592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204794112"/>
+        <c:crossAx val="204678272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1266,9 +1248,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204794112"/>
+        <c:axId val="204678272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="350000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1277,14 +1260,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204792576"/>
+        <c:crossAx val="231966592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205066240"/>
+        <c:axId val="204679808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1304,18 +1288,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205068160"/>
+        <c:crossAx val="204681984"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="205068160"/>
+        <c:axId val="204681984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1309,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205066240"/>
+        <c:crossAx val="204679808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1334,6 +1319,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1379,9 +1365,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$13:$H$23</c:f>
+              <c:f>DFA_R97_sched4!$G$15:$H$28</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -1407,6 +1393,15 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>maxDistLen:3</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1441,6 +1436,15 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1448,10 +1452,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$B$13:$B$23</c:f>
+              <c:f>DFA_R97_sched4!$B$15:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>23235</c:v>
                 </c:pt>
@@ -1484,6 +1488,15 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>16740</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148043</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>350368</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,9 +1519,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$13:$H$23</c:f>
+              <c:f>DFA_R97_sched4!$G$15:$H$28</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -1534,6 +1547,15 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>maxDistLen:3</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1568,6 +1590,15 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1575,10 +1606,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$C$13:$C$23</c:f>
+              <c:f>DFA_R97_sched4!$C$15:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>23235</c:v>
                 </c:pt>
@@ -1611,6 +1642,15 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>51109</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148043</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>350368</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1633,9 +1673,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$13:$H$23</c:f>
+              <c:f>DFA_R97_sched4!$G$15:$H$28</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -1661,6 +1701,15 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>maxDistLen:3</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1695,6 +1744,15 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1702,10 +1760,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$E$13:$E$23</c:f>
+              <c:f>DFA_R97_sched4!$E$15:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>306248</c:v>
                 </c:pt>
@@ -1738,6 +1796,15 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>223978</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1900233</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4772106</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>193827</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1754,8 +1821,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="205407744"/>
-        <c:axId val="205409280"/>
+        <c:axId val="204718464"/>
+        <c:axId val="204720000"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1776,10 +1843,10 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$D$13:$D$23</c:f>
+              <c:f>DFA_R97_sched4!$D$15:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
                 </c:pt>
@@ -1812,6 +1879,15 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1828,11 +1904,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="205421184"/>
-        <c:axId val="205419264"/>
+        <c:axId val="155321856"/>
+        <c:axId val="204721536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="205407744"/>
+        <c:axId val="204718464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1841,7 +1917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205409280"/>
+        <c:crossAx val="204720000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1849,9 +1925,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="205409280"/>
+        <c:axId val="204720000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="30000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1860,14 +1937,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205407744"/>
+        <c:crossAx val="204718464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205419264"/>
+        <c:axId val="204721536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1887,18 +1965,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205421184"/>
+        <c:crossAx val="155321856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="205421184"/>
+        <c:axId val="155321856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1907,7 +1986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205419264"/>
+        <c:crossAx val="204721536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1917,6 +1996,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1962,9 +2042,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$24:$H$34</c:f>
+              <c:f>DFA_R97_sched4!$G$29:$H$41</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -1990,6 +2070,12 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2024,6 +2110,12 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2031,10 +2123,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$B$24:$B$34</c:f>
+              <c:f>DFA_R97_sched4!$B$29:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>182367</c:v>
                 </c:pt>
@@ -2067,6 +2159,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>188241</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2089,9 +2187,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$24:$H$34</c:f>
+              <c:f>DFA_R97_sched4!$G$29:$H$41</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -2117,6 +2215,12 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2151,6 +2255,12 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2158,10 +2268,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$C$24:$C$34</c:f>
+              <c:f>DFA_R97_sched4!$C$29:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>22155</c:v>
                 </c:pt>
@@ -2194,6 +2304,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>16705</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2216,9 +2332,9 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$24:$H$34</c:f>
+              <c:f>DFA_R97_sched4!$G$29:$H$41</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>addAllPrefixesToS</c:v>
@@ -2244,6 +2360,12 @@
                   <c:pt idx="8">
                     <c:v>OneLocally</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>maxDistLen:2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ExtraStates:1</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2278,6 +2400,12 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Quotient</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>GoodSplit</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>OTree</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2285,10 +2413,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$E$24:$E$34</c:f>
+              <c:f>DFA_R97_sched4!$E$29:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>378173</c:v>
                 </c:pt>
@@ -2321,6 +2449,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>355563</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>152663</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2337,8 +2471,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="205461760"/>
-        <c:axId val="205471744"/>
+        <c:axId val="155385216"/>
+        <c:axId val="155395200"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2357,81 +2491,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>DFA_R97_sched4!$G$24:$H$34</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>addAllPrefixesToS</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>addAllSuffixesAfterLastStateToE</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>addSuffix1by1ToE</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>addSuffixAfterLastStateToE</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>addSuffixToE_binarySearch</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>AllGlobally</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>OneGlobally</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>OneLocally</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>L*</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>L*</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>L*</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>L*</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>L*</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>DT</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>OP</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>OP</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>OP</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>TTT</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Quotient</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DFA_R97_sched4!$D$24:$D$34</c:f>
+              <c:f>DFA_R97_sched4!$D$29:$D$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -2464,6 +2529,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2480,11 +2551,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="205474816"/>
-        <c:axId val="205473280"/>
+        <c:axId val="155410816"/>
+        <c:axId val="155396736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="205461760"/>
+        <c:axId val="155385216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2493,7 +2564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205471744"/>
+        <c:crossAx val="155395200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2501,7 +2572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="205471744"/>
+        <c:axId val="155395200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2512,14 +2583,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205461760"/>
+        <c:crossAx val="155385216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205473280"/>
+        <c:axId val="155396736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -2527,12 +2599,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205474816"/>
+        <c:crossAx val="155410816"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="205474816"/>
+        <c:axId val="155410816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2541,7 +2613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205473280"/>
+        <c:crossAx val="155396736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2551,6 +2623,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2575,7 +2648,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2965,10 +3038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,42 +3058,39 @@
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3037,22 +3107,19 @@
         <v>306248</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3069,22 +3136,19 @@
         <v>232284</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3101,22 +3165,19 @@
         <v>232183</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3133,22 +3194,19 @@
         <v>232389</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3165,22 +3223,19 @@
         <v>232651</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3197,19 +3252,16 @@
         <v>121988</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3226,22 +3278,19 @@
         <v>1104127</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3258,22 +3307,19 @@
         <v>275119</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3290,22 +3336,19 @@
         <v>226554</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3322,19 +3365,16 @@
         <v>45018</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3351,749 +3391,875 @@
         <v>223978</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>23235</v>
+        <v>148038</v>
       </c>
       <c r="C13">
-        <v>23235</v>
+        <v>148038</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1916339</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s">
         <v>12</v>
       </c>
-      <c r="E13">
-        <v>306248</v>
-      </c>
-      <c r="F13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L13" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
-        <v>18654</v>
+        <v>14643</v>
       </c>
       <c r="C14">
-        <v>18654</v>
+        <v>27113</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>232284</v>
+        <v>193827</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>50</v>
-      </c>
-      <c r="L14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15">
-        <v>18640</v>
+        <v>23235</v>
       </c>
       <c r="C15">
-        <v>18640</v>
+        <v>23235</v>
       </c>
       <c r="D15">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E15">
-        <v>232183</v>
+        <v>306248</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
-      </c>
-      <c r="L15" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16">
-        <v>18670</v>
+        <v>18654</v>
       </c>
       <c r="C16">
-        <v>18670</v>
+        <v>18654</v>
       </c>
       <c r="D16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16">
-        <v>232389</v>
+        <v>232284</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
-      </c>
-      <c r="L16" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17">
-        <v>18699</v>
+        <v>18640</v>
       </c>
       <c r="C17">
-        <v>18699</v>
+        <v>18640</v>
       </c>
       <c r="D17">
         <v>16</v>
       </c>
       <c r="E17">
-        <v>232651</v>
+        <v>232183</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18">
-        <v>11805</v>
+        <v>18670</v>
       </c>
       <c r="C18">
-        <v>11805</v>
+        <v>18670</v>
       </c>
       <c r="D18">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="E18">
-        <v>121988</v>
+        <v>232389</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
       </c>
       <c r="I18" t="s">
-        <v>50</v>
-      </c>
-      <c r="L18" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19">
-        <v>63670</v>
+        <v>18699</v>
       </c>
       <c r="C19">
-        <v>63670</v>
+        <v>18699</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E19">
-        <v>1104127</v>
+        <v>232651</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>50</v>
-      </c>
-      <c r="L19" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20">
-        <v>21736</v>
+        <v>11805</v>
       </c>
       <c r="C20">
-        <v>21736</v>
+        <v>11805</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="E20">
-        <v>275119</v>
+        <v>121988</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I20" t="s">
-        <v>50</v>
-      </c>
-      <c r="L20" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21">
-        <v>18322</v>
+        <v>63670</v>
       </c>
       <c r="C21">
-        <v>18322</v>
+        <v>63670</v>
       </c>
       <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>1104127</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s">
         <v>18</v>
       </c>
-      <c r="E21">
-        <v>226554</v>
-      </c>
-      <c r="F21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" t="s">
-        <v>46</v>
-      </c>
       <c r="H21" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>50</v>
-      </c>
-      <c r="L21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22">
-        <v>3606</v>
+        <v>21736</v>
       </c>
       <c r="C22">
-        <v>3606</v>
+        <v>21736</v>
       </c>
       <c r="D22">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>45018</v>
+        <v>275119</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="H22" t="s">
+        <v>20</v>
       </c>
       <c r="I22" t="s">
-        <v>50</v>
-      </c>
-      <c r="L22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23">
-        <v>16740</v>
+        <v>18322</v>
       </c>
       <c r="C23">
-        <v>51109</v>
+        <v>18322</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E23">
-        <v>223978</v>
+        <v>226554</v>
       </c>
       <c r="F23" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G23" t="s">
-        <v>54</v>
+        <v>18</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
       </c>
       <c r="I23" t="s">
-        <v>50</v>
-      </c>
-      <c r="L23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24">
-        <v>182367</v>
+        <v>3606</v>
       </c>
       <c r="C24">
-        <v>22155</v>
+        <v>3606</v>
       </c>
       <c r="D24">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="E24">
-        <v>378173</v>
+        <v>45018</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I24" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" t="s">
-        <v>52</v>
-      </c>
-      <c r="L24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25">
-        <v>186418</v>
+        <v>16740</v>
       </c>
       <c r="C25">
-        <v>20985</v>
+        <v>51109</v>
       </c>
       <c r="D25">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>357692</v>
+        <v>223978</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" t="s">
-        <v>52</v>
-      </c>
-      <c r="L25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26">
-        <v>186646</v>
+        <v>148043</v>
       </c>
       <c r="C26">
-        <v>20970</v>
+        <v>148043</v>
       </c>
       <c r="D26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>372640</v>
+        <v>1900233</v>
       </c>
       <c r="F26" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H26" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="I26" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" t="s">
-        <v>52</v>
-      </c>
-      <c r="L26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27">
-        <v>192327</v>
+        <v>350368</v>
       </c>
       <c r="C27">
-        <v>21004</v>
+        <v>350368</v>
       </c>
       <c r="D27">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>361742</v>
+        <v>4772106</v>
       </c>
       <c r="F27" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="I27" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" t="s">
-        <v>52</v>
-      </c>
-      <c r="L27" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28">
-        <v>192361</v>
+        <v>14643</v>
       </c>
       <c r="C28">
-        <v>21038</v>
+        <v>27113</v>
       </c>
       <c r="D28">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>361742</v>
+        <v>193827</v>
       </c>
       <c r="F28" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G28" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H28" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="I28" t="s">
-        <v>51</v>
-      </c>
-      <c r="J28" t="s">
-        <v>52</v>
-      </c>
-      <c r="L28" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29">
-        <v>562049</v>
+        <v>182367</v>
       </c>
       <c r="C29">
-        <v>11667</v>
+        <v>22155</v>
       </c>
       <c r="D29">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="E29">
-        <v>356088</v>
+        <v>378173</v>
       </c>
       <c r="F29" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G29" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="H29" t="s">
+        <v>11</v>
       </c>
       <c r="I29" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="J29" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30">
-        <v>276871</v>
+        <v>186418</v>
       </c>
       <c r="C30">
-        <v>116094</v>
+        <v>20985</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E30">
-        <v>698416</v>
+        <v>357692</v>
       </c>
       <c r="F30" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="I30" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="J30" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31">
-        <v>182512</v>
+        <v>186646</v>
       </c>
       <c r="C31">
-        <v>21735</v>
+        <v>20970</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E31">
-        <v>355596</v>
+        <v>372640</v>
       </c>
       <c r="F31" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="I31" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="J31" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32">
-        <v>284397</v>
+        <v>192327</v>
       </c>
       <c r="C32">
-        <v>18322</v>
+        <v>21004</v>
       </c>
       <c r="D32">
         <v>18</v>
       </c>
       <c r="E32">
-        <v>355580</v>
+        <v>361742</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G32" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="I32" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="J32" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33">
-        <v>579645</v>
+        <v>192361</v>
       </c>
       <c r="C33">
-        <v>3640</v>
+        <v>21038</v>
       </c>
       <c r="D33">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="E33">
-        <v>358356</v>
+        <v>361742</v>
       </c>
       <c r="F33" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="G33" t="s">
-        <v>55</v>
+        <v>10</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
       </c>
       <c r="I33" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="J33" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34">
-        <v>188241</v>
+        <v>562049</v>
       </c>
       <c r="C34">
-        <v>16705</v>
+        <v>11667</v>
       </c>
       <c r="D34">
+        <v>96</v>
+      </c>
+      <c r="E34">
+        <v>356088</v>
+      </c>
+      <c r="F34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" t="s">
+        <v>23</v>
+      </c>
+      <c r="J34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>276871</v>
+      </c>
+      <c r="C35">
+        <v>116094</v>
+      </c>
+      <c r="D35">
         <v>4</v>
       </c>
-      <c r="E34">
-        <v>355563</v>
-      </c>
-      <c r="F34" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" t="s">
-        <v>54</v>
-      </c>
-      <c r="I34" t="s">
-        <v>51</v>
-      </c>
-      <c r="J34" t="s">
-        <v>52</v>
+      <c r="E35">
+        <v>698416</v>
+      </c>
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36">
-        <v>350368</v>
+        <v>182512</v>
       </c>
       <c r="C36">
-        <v>350368</v>
+        <v>21735</v>
       </c>
       <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>355596</v>
+      </c>
+      <c r="F36" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>284397</v>
+      </c>
+      <c r="C37">
+        <v>18322</v>
+      </c>
+      <c r="D37">
+        <v>18</v>
+      </c>
+      <c r="E37">
+        <v>355580</v>
+      </c>
+      <c r="F37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>579645</v>
+      </c>
+      <c r="C38">
+        <v>3640</v>
+      </c>
+      <c r="D38">
+        <v>92</v>
+      </c>
+      <c r="E38">
+        <v>358356</v>
+      </c>
+      <c r="F38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" t="s">
+        <v>23</v>
+      </c>
+      <c r="J38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>188241</v>
+      </c>
+      <c r="C39">
+        <v>16705</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>355563</v>
+      </c>
+      <c r="F39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" t="s">
+        <v>23</v>
+      </c>
+      <c r="J39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>149721</v>
+      </c>
+      <c r="C40">
+        <v>149721</v>
+      </c>
+      <c r="D40">
         <v>0</v>
       </c>
-      <c r="E36">
-        <v>4772106</v>
-      </c>
-      <c r="F36" t="s">
-        <v>53</v>
-      </c>
-      <c r="G36" t="s">
-        <v>57</v>
-      </c>
-      <c r="H36" t="s">
-        <v>58</v>
-      </c>
-      <c r="I36" t="s">
-        <v>50</v>
-      </c>
-      <c r="L36" t="s">
-        <v>56</v>
+      <c r="E40">
+        <v>152663</v>
+      </c>
+      <c r="F40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" t="s">
+        <v>23</v>
+      </c>
+      <c r="J40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>14643</v>
+      </c>
+      <c r="C41">
+        <v>27113</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>27113</v>
+      </c>
+      <c r="F41" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" t="s">
+        <v>23</v>
+      </c>
+      <c r="J41" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>